<commit_message>
exists and update repository functions
</commit_message>
<xml_diff>
--- a/xlsx_files/samplefile.xlsx
+++ b/xlsx_files/samplefile.xlsx
@@ -2,9 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="SampleList" sheetId="1" r:id="rId1"/>
@@ -36,9 +36,6 @@
     <t>available</t>
   </si>
   <si>
-    <t>moloko</t>
-  </si>
-  <si>
     <t>true</t>
   </si>
   <si>
@@ -51,13 +48,16 @@
     <t>false</t>
   </si>
   <si>
-    <t>cucus</t>
+    <t>NEWMOLOKO</t>
+  </si>
+  <si>
+    <t>cucusNEW</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -372,12 +372,12 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -394,12 +394,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C2">
         <v>89</v>
@@ -408,15 +408,15 @@
         <v>223</v>
       </c>
       <c r="E2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3">
         <v>114</v>
@@ -425,15 +425,15 @@
         <v>89</v>
       </c>
       <c r="E3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4">
         <v>40</v>
@@ -442,12 +442,12 @@
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
@@ -459,7 +459,7 @@
         <v>123</v>
       </c>
       <c r="E5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>